<commit_message>
add functions to reflect new functions of xmllib (#62)
</commit_message>
<xml_diff>
--- a/daschland_ontology/json_header.xlsx
+++ b/daschland_ontology/json_header.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6CC743-92E4-2242-8042-4977508341B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A1EB16-7F59-014C-9BCB-248C5E45EAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="500" windowWidth="76480" windowHeight="31180" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44620" yWindow="500" windowWidth="32180" windowHeight="31180" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>username</t>
   </si>
@@ -311,12 +311,15 @@
   <si>
     <t>http://rdfh.ch/licenses/ai-generated</t>
   </si>
+  <si>
+    <t>http://rdfh.ch/licenses/cc-0-1.0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +388,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -414,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -461,6 +470,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -16259,7 +16269,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16287,8 +16297,10 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
+    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>

</xml_diff>

<commit_message>
remove user passwords from Excel and project JSON (DEV-5492) (#79)
</commit_message>
<xml_diff>
--- a/daschland_ontology/json_header.xlsx
+++ b/daschland_ontology/json_header.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/daschland-scripts/daschland_ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2432AF33-F570-A845-8325-1876E547046E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19753C7-EEBC-4E44-82F8-4B804657A967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44620" yWindow="500" windowWidth="32180" windowHeight="31180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44620" yWindow="620" windowWidth="32180" windowHeight="30260" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
   <si>
     <t>username</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Liddell</t>
   </si>
   <si>
-    <t>alice4322</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
   </si>
   <si>
     <t>Wonderland</t>
-  </si>
-  <si>
-    <t>alice7652</t>
   </si>
   <si>
     <t>de</t>
@@ -109,9 +103,6 @@
     <t>Rabbit</t>
   </si>
   <si>
-    <t>alice8711</t>
-  </si>
-  <si>
     <t>fr</t>
   </si>
   <si>
@@ -125,9 +116,6 @@
   </si>
   <si>
     <t>Cat</t>
-  </si>
-  <si>
-    <t>alice9548</t>
   </si>
   <si>
     <t>projectadmin</t>
@@ -782,8 +770,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -795,10 +783,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -827,42 +815,42 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B4" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B5" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B6" s="19" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1893,16 +1881,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1929,16 +1917,16 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6956,19 +6944,19 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="6"/>
@@ -6994,16 +6982,16 @@
     </row>
     <row r="2" spans="1:26" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E2" s="11"/>
     </row>
@@ -14016,7 +14004,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -14046,107 +14034,107 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15130,7 +15118,9 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15197,83 +15187,75 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16291,27 +16273,27 @@
   <sheetData>
     <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">

</xml_diff>